<commit_message>
Price harvester rework - adjusting responsibilities to take some functionality away from client program (if harvester was to be kept separate). Fixing issues causing price times to reset.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -406,19 +406,19 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -426,25 +426,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
       </c>
       <c r="I1" t="s">
         <v>8</v>
@@ -455,29 +455,29 @@
         <v>43122</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H2">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I2">
         <f>SUM(B2:H2)</f>
-        <v>8</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -485,29 +485,29 @@
         <v>43129</v>
       </c>
       <c r="B3">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
         <v>5</v>
       </c>
-      <c r="C3">
+      <c r="F3">
         <v>5</v>
       </c>
-      <c r="D3">
+      <c r="G3">
+        <v>9</v>
+      </c>
+      <c r="H3">
         <v>7</v>
-      </c>
-      <c r="E3">
-        <v>7</v>
-      </c>
-      <c r="F3">
-        <v>6</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
       </c>
       <c r="I3">
         <f>SUM(B3:H3)</f>
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -515,23 +515,32 @@
         <v>43136</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>9</v>
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
       </c>
       <c r="I4">
         <f t="shared" ref="I4:I18" si="0">SUM(B4:H4)</f>
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43143</v>
       </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
       <c r="I5">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -541,6 +550,12 @@
       <c r="A6" s="1">
         <v>43150</v>
       </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
       <c r="I6">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -550,6 +565,12 @@
       <c r="A7" s="1">
         <v>43157</v>
       </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
       <c r="I7">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -559,6 +580,12 @@
       <c r="A8" s="1">
         <v>43164</v>
       </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
       <c r="I8">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -568,6 +595,12 @@
       <c r="A9" s="1">
         <v>43171</v>
       </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
       <c r="I9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -577,6 +610,12 @@
       <c r="A10" s="1">
         <v>43178</v>
       </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
       <c r="I10">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -586,6 +625,12 @@
       <c r="A11" s="1">
         <v>43185</v>
       </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
       <c r="I11">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -595,6 +640,12 @@
       <c r="A12" s="1">
         <v>43192</v>
       </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
       <c r="I12">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -604,6 +655,12 @@
       <c r="A13" s="1">
         <v>43199</v>
       </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
       <c r="I13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -613,6 +670,12 @@
       <c r="A14" s="1">
         <v>43206</v>
       </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
       <c r="I14">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -622,6 +685,12 @@
       <c r="A15" s="1">
         <v>43213</v>
       </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
       <c r="I15">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -631,6 +700,12 @@
       <c r="A16" s="1">
         <v>43220</v>
       </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
       <c r="I16">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -640,6 +715,12 @@
       <c r="A17" s="1">
         <v>43227</v>
       </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
       <c r="I17">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -648,6 +729,12 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43234</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
       </c>
       <c r="I18">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Created JUnit tests for entirety of project. Finished JUnit testing for model (and fixed issues uncovered).
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -406,7 +406,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,29 +455,29 @@
         <v>43122</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="D2">
         <v>2</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>5.25</v>
       </c>
       <c r="F2">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="G2">
-        <v>7</v>
+        <v>6.5</v>
       </c>
       <c r="H2">
-        <v>7</v>
+        <v>7.5</v>
       </c>
       <c r="I2">
         <f>SUM(B2:H2)</f>
-        <v>32</v>
+        <v>32.75</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -485,7 +485,7 @@
         <v>43129</v>
       </c>
       <c r="B3">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -494,20 +494,20 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>5.25</v>
       </c>
       <c r="F3">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="G3">
-        <v>9</v>
+        <v>8.5</v>
       </c>
       <c r="H3">
-        <v>7</v>
+        <v>7.5</v>
       </c>
       <c r="I3">
         <f>SUM(B3:H3)</f>
-        <v>32</v>
+        <v>33.25</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -515,20 +515,23 @@
         <v>43136</v>
       </c>
       <c r="B4">
-        <v>7</v>
+        <v>7.5</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>5.75</v>
+      </c>
+      <c r="F4">
+        <v>7.25</v>
       </c>
       <c r="I4">
         <f t="shared" ref="I4:I18" si="0">SUM(B4:H4)</f>
-        <v>9</v>
+        <v>21.75</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished JUnit testing. Started work on prediction algorithm.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -406,7 +406,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,9 +529,12 @@
       <c r="F4">
         <v>7.25</v>
       </c>
+      <c r="G4">
+        <v>8</v>
+      </c>
       <c r="I4">
         <f t="shared" ref="I4:I18" si="0">SUM(B4:H4)</f>
-        <v>21.75</v>
+        <v>29.75</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Created safe casting helper to remove reliance on object arrays. Reworked classes to use new helper. In position to be able to make GOFAI prediction algorithms for testing.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -406,7 +406,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,11 +530,14 @@
         <v>7.25</v>
       </c>
       <c r="G4">
-        <v>8</v>
+        <v>7.5</v>
+      </c>
+      <c r="H4">
+        <v>4.25</v>
       </c>
       <c r="I4">
         <f t="shared" ref="I4:I18" si="0">SUM(B4:H4)</f>
-        <v>29.75</v>
+        <v>33.5</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated documentation. Started GOFAI prediction algorithm comparisons.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -406,7 +406,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,11 +533,11 @@
         <v>7.5</v>
       </c>
       <c r="H4">
-        <v>4.25</v>
+        <v>7.25</v>
       </c>
       <c r="I4">
         <f t="shared" ref="I4:I18" si="0">SUM(B4:H4)</f>
-        <v>33.5</v>
+        <v>36.5</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Calculating mean predicted change and error using 1-20 previous prices. It appears more prices = lower predicted change AND lower error.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -406,7 +406,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,6 +544,9 @@
       <c r="A5" s="1">
         <v>43143</v>
       </c>
+      <c r="B5">
+        <v>5.25</v>
+      </c>
       <c r="C5">
         <v>0</v>
       </c>
@@ -552,7 +555,7 @@
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5.25</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Attempting to create and deploy API. Might need to reinstall VS + Oracle at home. Basic Java endpoint controllers likely working - need to get VS working to test.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -406,7 +406,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,9 +553,15 @@
       <c r="D5">
         <v>0</v>
       </c>
+      <c r="E5">
+        <v>3.5</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>5.25</v>
+        <v>11.75</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
GOT API WORKING! Start to work through 2 modes - database mode and database free mode.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -406,7 +406,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,11 +557,14 @@
         <v>3.5</v>
       </c>
       <c r="F5">
-        <v>3</v>
+        <v>8</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>11.75</v>
+        <v>17.75</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Parsing Currencies from Oracle to initialise application. Attemping to post live ExchangeRates to Oracle but getting 415 -- i *think* i need to crop doubles to suitable sizes.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -406,7 +406,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,14 +557,14 @@
         <v>3.5</v>
       </c>
       <c r="F5">
-        <v>8</v>
+        <v>8.25</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>7.75</v>
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>17.75</v>
+        <v>24.75</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Synchronising after editing highlights & hours worked log. Need to remake project with maven to handle dependencies.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\Final Project\PRCO304\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\FinalProject\PRCO304\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -406,7 +406,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,9 +562,12 @@
       <c r="G5">
         <v>7.75</v>
       </c>
+      <c r="H5">
+        <v>7.25</v>
+      </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>24.75</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finally fixed Post. Gson was parsing LDT in a way that Oracle / EF API didn't understand/like. Currently posts live prices only...
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -406,7 +406,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,6 +574,9 @@
       <c r="A6" s="1">
         <v>43150</v>
       </c>
+      <c r="B6">
+        <v>8.25</v>
+      </c>
       <c r="C6">
         <v>0</v>
       </c>
@@ -582,7 +585,7 @@
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.25</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Working on posting historic data - need to implement batch post solution at API endpoint (or spam api with single prices D:)
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -403,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D973A54-FCD3-4BD0-A506-47414655087F}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,7 +575,7 @@
         <v>43150</v>
       </c>
       <c r="B6">
-        <v>8.25</v>
+        <v>9.25</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -585,7 +585,7 @@
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>8.25</v>
+        <v>9.25</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -766,6 +766,12 @@
       <c r="I18">
         <f t="shared" si="0"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <f>SUM(I2:I18)</f>
+        <v>143.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Initial load working. Need to rework historic posting. Logic to implement underlined in function. Also need to work out how to do a PUT (and DELETE) using a compound key of currency + timestamp.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -406,7 +406,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,9 +583,12 @@
       <c r="D6">
         <v>0</v>
       </c>
+      <c r="E6">
+        <v>5.5</v>
+      </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>9.25</v>
+        <v>14.75</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -771,7 +774,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f>SUM(I2:I18)</f>
-        <v>143.75</v>
+        <v>149.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Had to change API for GET/RATE/ and PUT/RATE/. Seems to be working. Need to devise scheme to not pull from GDAX if price pulled from Database.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -406,7 +406,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,11 +584,14 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>5.5</v>
+        <v>6.5</v>
+      </c>
+      <c r="F6">
+        <v>7.5</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>14.75</v>
+        <v>23.25</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -774,7 +777,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f>SUM(I2:I18)</f>
-        <v>149.25</v>
+        <v>157.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added get/exchangerate/{currency} to api to reduce java processing of data. Working on gap filling harvester logic.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -406,7 +406,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,9 +589,12 @@
       <c r="F6">
         <v>7.5</v>
       </c>
+      <c r="G6">
+        <v>8.25</v>
+      </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>23.25</v>
+        <v>31.5</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -777,7 +780,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f>SUM(I2:I18)</f>
-        <v>157.75</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Gap fill mode [appears to be] working. 10k prices harvested. Finished hours worked and highlight for week. Pushing before beginning work on spoof trading.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -406,7 +406,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,7 +575,7 @@
         <v>43150</v>
       </c>
       <c r="B6">
-        <v>9.25</v>
+        <v>8.25</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -592,9 +592,12 @@
       <c r="G6">
         <v>8.25</v>
       </c>
+      <c r="H6">
+        <v>6.25</v>
+      </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>31.5</v>
+        <v>36.75</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -780,7 +783,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f>SUM(I2:I18)</f>
-        <v>166</v>
+        <v>171.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Streamlined historic collection. Started work on trading bot in preparation for decision making assessment.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,6 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\FinalProject\PRCO304\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B5E72E-B1B7-4FD9-AA13-BB58B6484E98}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{B9A26406-05FA-4FD5-AABB-5F887CCEE042}"/>
   </bookViews>
@@ -406,7 +407,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,6 +605,9 @@
       <c r="A7" s="1">
         <v>43157</v>
       </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
       <c r="C7">
         <v>0</v>
       </c>
@@ -612,7 +616,7 @@
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -783,7 +787,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f>SUM(I2:I18)</f>
-        <v>171.25</v>
+        <v>175.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Various design work for Marco. Started work on trader before GOFAI options can be tested.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\FinalProject\PRCO304\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B5E72E-B1B7-4FD9-AA13-BB58B6484E98}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21AB1DF5-60DC-4900-9C7A-A354CD8C9C87}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{B9A26406-05FA-4FD5-AABB-5F887CCEE042}"/>
   </bookViews>
@@ -407,7 +407,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,7 +606,7 @@
         <v>43157</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>6.75</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -616,7 +616,7 @@
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>6.75</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -787,7 +787,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f>SUM(I2:I18)</f>
-        <v>175.25</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Autotrade mode work in place. Need to develop system to fill gaps.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\FinalProject\PRCO304\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21AB1DF5-60DC-4900-9C7A-A354CD8C9C87}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B736F60-DF81-44E9-B511-8DF7429F5850}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{B9A26406-05FA-4FD5-AABB-5F887CCEE042}"/>
   </bookViews>
@@ -407,7 +407,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,9 +614,12 @@
       <c r="D7">
         <v>0</v>
       </c>
+      <c r="E7">
+        <v>2.25</v>
+      </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>6.75</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -787,7 +790,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f>SUM(I2:I18)</f>
-        <v>178</v>
+        <v>180.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Price estimation logic added for minutes with no trade data on gdax. Continuation of autotrading logic.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\FinalProject\PRCO304\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B736F60-DF81-44E9-B511-8DF7429F5850}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{718E8411-4E7B-44AF-B322-B10D92775119}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{B9A26406-05FA-4FD5-AABB-5F887CCEE042}"/>
   </bookViews>
@@ -407,7 +407,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,11 +615,11 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>2.25</v>
+        <v>4.5</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>11.25</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -790,7 +790,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f>SUM(I2:I18)</f>
-        <v>180.25</v>
+        <v>182.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug fix + Work on testing gofai methods.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\FinalProject\PRCO304\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{718E8411-4E7B-44AF-B322-B10D92775119}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD7CFA3-15CC-4152-8027-AEE41683785A}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{B9A26406-05FA-4FD5-AABB-5F887CCEE042}"/>
   </bookViews>
@@ -407,7 +407,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,9 +617,12 @@
       <c r="E7">
         <v>4.5</v>
       </c>
+      <c r="F7">
+        <v>6.25</v>
+      </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>11.25</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -790,7 +793,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f>SUM(I2:I18)</f>
-        <v>182.5</v>
+        <v>188.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Anomalous bug fixing. Working towards getting spoof trading working.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\FinalProject\PRCO304\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD7CFA3-15CC-4152-8027-AEE41683785A}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57174F60-23BA-49FA-85A3-06142E8A7E4C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{B9A26406-05FA-4FD5-AABB-5F887CCEE042}"/>
   </bookViews>
@@ -407,7 +407,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,11 +618,14 @@
         <v>4.5</v>
       </c>
       <c r="F7">
-        <v>6.25</v>
+        <v>6.75</v>
+      </c>
+      <c r="G7">
+        <v>7.75</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>17.5</v>
+        <v>25.75</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -793,7 +796,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f>SUM(I2:I18)</f>
-        <v>188.75</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed trading issue (no longer produces NaN). Localised connected/failed to connect to database bug as occuring when database has current data (i.e. 0 gaps)
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\FinalProject\PRCO304\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57174F60-23BA-49FA-85A3-06142E8A7E4C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C306BC30-7630-4955-84B6-BB58C79A3E71}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{B9A26406-05FA-4FD5-AABB-5F887CCEE042}"/>
   </bookViews>
@@ -407,7 +407,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,9 +623,12 @@
       <c r="G7">
         <v>7.75</v>
       </c>
+      <c r="H7">
+        <v>3.25</v>
+      </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>25.75</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -796,7 +799,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f>SUM(I2:I18)</f>
-        <v>197</v>
+        <v>200.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Historic prices appear to need offsetting by -1 minute. Look more thoroughly tomorrow.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\FinalProject\PRCO304\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C306BC30-7630-4955-84B6-BB58C79A3E71}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48ACDBF0-46D3-4E5A-B4F5-DE0FDB750255}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{B9A26406-05FA-4FD5-AABB-5F887CCEE042}"/>
   </bookViews>
@@ -407,7 +407,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,11 +624,11 @@
         <v>7.75</v>
       </c>
       <c r="H7">
-        <v>3.25</v>
+        <v>6.25</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -799,7 +799,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f>SUM(I2:I18)</f>
-        <v>200.25</v>
+        <v>203.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Various bug fixes. Added bug log to readme file.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\FinalProject\PRCO304\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48ACDBF0-46D3-4E5A-B4F5-DE0FDB750255}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E746676-0A72-4DF6-B7C6-B58A3DE78F39}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{B9A26406-05FA-4FD5-AABB-5F887CCEE042}"/>
   </bookViews>
@@ -407,7 +407,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,6 +635,9 @@
       <c r="A8" s="1">
         <v>43164</v>
       </c>
+      <c r="B8">
+        <v>4.25</v>
+      </c>
       <c r="C8">
         <v>0</v>
       </c>
@@ -643,7 +646,7 @@
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.25</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -799,7 +802,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f>SUM(I2:I18)</f>
-        <v>203.25</v>
+        <v>207.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GUI integration started. Bugfixing/tracing: dumpDuplicates found as source of bug.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\FinalProject\PRCO304\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E746676-0A72-4DF6-B7C6-B58A3DE78F39}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EDBAB7B-182E-43B6-8D53-5513AB01E4B7}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{B9A26406-05FA-4FD5-AABB-5F887CCEE042}"/>
   </bookViews>
@@ -407,7 +407,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,9 +644,12 @@
       <c r="D8">
         <v>0</v>
       </c>
+      <c r="E8">
+        <v>6.5</v>
+      </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>4.25</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -802,7 +805,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f>SUM(I2:I18)</f>
-        <v>207.5</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed concurrency issue by switching to single collection thread. Still have a few bugs to resolve with it.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\FinalProject\PRCO304\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EDBAB7B-182E-43B6-8D53-5513AB01E4B7}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE88C373-4CB9-47F1-A430-1B22F90A7F69}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{B9A26406-05FA-4FD5-AABB-5F887CCEE042}"/>
   </bookViews>
@@ -407,7 +407,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,9 +647,12 @@
       <c r="E8">
         <v>6.5</v>
       </c>
+      <c r="F8">
+        <v>7.25</v>
+      </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>10.75</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -805,7 +808,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f>SUM(I2:I18)</f>
-        <v>214</v>
+        <v>221.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed collector thread. Need to halt historic collection once second lap is completed.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\FinalProject\PRCO304\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE88C373-4CB9-47F1-A430-1B22F90A7F69}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC770528-FD37-4F6E-8F10-FD469386BEBD}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{B9A26406-05FA-4FD5-AABB-5F887CCEE042}"/>
   </bookViews>
@@ -407,7 +407,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,9 +650,12 @@
       <c r="F8">
         <v>7.25</v>
       </c>
+      <c r="G8">
+        <v>6.5</v>
+      </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>24.5</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -808,7 +811,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f>SUM(I2:I18)</f>
-        <v>221.25</v>
+        <v>227.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mostly GUI work. Added some functionality to display currencies and timestamps in a user friendly way.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\FinalProject\PRCO304\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC770528-FD37-4F6E-8F10-FD469386BEBD}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91D555B-8053-4C2A-A6F1-C63BB4620625}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{B9A26406-05FA-4FD5-AABB-5F887CCEE042}"/>
   </bookViews>
@@ -407,7 +407,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,11 +651,11 @@
         <v>7.25</v>
       </c>
       <c r="G8">
-        <v>6.5</v>
+        <v>8.5</v>
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>24.5</v>
+        <v>26.5</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -811,7 +811,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f>SUM(I2:I18)</f>
-        <v>227.75</v>
+        <v>229.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GOFAI predictions now being displayed on GUI. Added text to indicate to user where missing functionality is missing by intention, not error.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\FinalProject\PRCO304\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91D555B-8053-4C2A-A6F1-C63BB4620625}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27CE84AE-C886-4498-BC18-EF0467C7B20E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{B9A26406-05FA-4FD5-AABB-5F887CCEE042}"/>
   </bookViews>
@@ -407,7 +407,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,9 +653,12 @@
       <c r="G8">
         <v>8.5</v>
       </c>
+      <c r="H8">
+        <v>6.5</v>
+      </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>26.5</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -811,7 +814,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f>SUM(I2:I18)</f>
-        <v>229.75</v>
+        <v>236.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GUI work. Logic improvements. Bug fixing. Push for demo.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\FinalProject\PRCO304\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27CE84AE-C886-4498-BC18-EF0467C7B20E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB4DA78-1661-414D-B19C-A4F738FA61C9}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{B9A26406-05FA-4FD5-AABB-5F887CCEE042}"/>
   </bookViews>
@@ -407,7 +407,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,6 +665,9 @@
       <c r="A9" s="1">
         <v>43171</v>
       </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
       <c r="C9">
         <v>0</v>
       </c>
@@ -673,7 +676,7 @@
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -814,7 +817,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f>SUM(I2:I18)</f>
-        <v>236.25</v>
+        <v>243.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed various issues including skipping minutes within gaps where data is missing.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\FinalProject\PRCO304\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB4DA78-1661-414D-B19C-A4F738FA61C9}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85EA27D-96C3-4000-836C-B5124295FA59}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{B9A26406-05FA-4FD5-AABB-5F887CCEE042}"/>
   </bookViews>
@@ -407,7 +407,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,9 +674,12 @@
       <c r="D9">
         <v>0</v>
       </c>
+      <c r="E9">
+        <v>5.75</v>
+      </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>12.75</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -817,7 +820,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f>SUM(I2:I18)</f>
-        <v>243.25</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Benchmarking completed. Fixed newly discovered issue with gap filler. Need to purge and refill database due to potentially corrupted data [caused by gap filler bug]. Benchmarking GUI completed (ish).
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\FinalProject\PRCO304\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85EA27D-96C3-4000-836C-B5124295FA59}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8328BFA-BB95-4622-AE87-292536584202}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{B9A26406-05FA-4FD5-AABB-5F887CCEE042}"/>
   </bookViews>
@@ -407,7 +407,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,9 +677,12 @@
       <c r="E9">
         <v>5.75</v>
       </c>
+      <c r="F9">
+        <v>5.25</v>
+      </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>12.75</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -820,7 +823,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f>SUM(I2:I18)</f>
-        <v>249</v>
+        <v>254.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working towards live trading. Collector now holds predictions to make future predictions faster.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\FinalProject\PRCO304\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8328BFA-BB95-4622-AE87-292536584202}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C8245C5-4555-479D-BBA2-B8851F1FFD2F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{B9A26406-05FA-4FD5-AABB-5F887CCEE042}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Week Commencing</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Easter</t>
   </si>
 </sst>
 </file>
@@ -404,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D973A54-FCD3-4BD0-A506-47414655087F}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,7 +425,7 @@
     <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -451,7 +454,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43122</v>
       </c>
@@ -481,7 +484,7 @@
         <v>32.75</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43129</v>
       </c>
@@ -511,7 +514,7 @@
         <v>33.25</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43136</v>
       </c>
@@ -541,7 +544,7 @@
         <v>36.5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43143</v>
       </c>
@@ -571,7 +574,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43150</v>
       </c>
@@ -601,7 +604,7 @@
         <v>36.75</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43157</v>
       </c>
@@ -631,7 +634,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43164</v>
       </c>
@@ -661,7 +664,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43171</v>
       </c>
@@ -678,14 +681,14 @@
         <v>5.75</v>
       </c>
       <c r="F9">
-        <v>5.25</v>
+        <v>7.25</v>
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43178</v>
       </c>
@@ -699,26 +702,50 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43185</v>
       </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
       <c r="I11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43192</v>
       </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
       <c r="C12">
         <v>0</v>
       </c>
@@ -729,8 +756,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43199</v>
       </c>
@@ -745,7 +775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43206</v>
       </c>
@@ -760,7 +790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43213</v>
       </c>
@@ -775,7 +805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43220</v>
       </c>
@@ -823,7 +853,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f>SUM(I2:I18)</f>
-        <v>254.25</v>
+        <v>256.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Live predictions made and nearly finished real trader.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\FinalProject\PRCO304\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C8245C5-4555-479D-BBA2-B8851F1FFD2F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3542BD-5309-44D6-97E4-4E93BC362995}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{B9A26406-05FA-4FD5-AABB-5F887CCEE042}"/>
   </bookViews>
@@ -410,7 +410,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,9 +683,12 @@
       <c r="F9">
         <v>7.25</v>
       </c>
+      <c r="G9">
+        <v>6.75</v>
+      </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>26.75</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -853,7 +856,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f>SUM(I2:I18)</f>
-        <v>256.25</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug fixes. Various logic modifications to allow user to pick which GOFAI algorithm to trade with. Development of GUI and trade mode.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\FinalProject\PRCO304\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3542BD-5309-44D6-97E4-4E93BC362995}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131DF6C3-FC17-4B94-81FD-B45610D8E048}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{B9A26406-05FA-4FD5-AABB-5F887CCEE042}"/>
   </bookViews>
@@ -410,7 +410,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,9 +686,12 @@
       <c r="G9">
         <v>6.75</v>
       </c>
+      <c r="H9">
+        <v>5.25</v>
+      </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>26.75</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -856,7 +859,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f>SUM(I2:I18)</f>
-        <v>263</v>
+        <v>268.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Spoof trading appears to be fully functional. Need to apply taker fee before live trading. Fixed issue with GUI expanding.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\FinalProject\PRCO304\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131DF6C3-FC17-4B94-81FD-B45610D8E048}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC65F7D4-BBBB-4A49-8AD0-8628A0367B7C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{B9A26406-05FA-4FD5-AABB-5F887CCEE042}"/>
   </bookViews>
@@ -410,7 +410,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,6 +698,9 @@
       <c r="A10" s="1">
         <v>43178</v>
       </c>
+      <c r="B10">
+        <v>4.25</v>
+      </c>
       <c r="C10">
         <v>0</v>
       </c>
@@ -706,7 +709,7 @@
       </c>
       <c r="I10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.25</v>
       </c>
       <c r="J10" t="s">
         <v>9</v>
@@ -859,7 +862,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f>SUM(I2:I18)</f>
-        <v>268.25</v>
+        <v>272.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started basis for integrating GDAX API trades. Created JUnit tests & imported prior implemented tests. Need to import JUnit Library and finish tests.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\FinalProject\PRCO304\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC65F7D4-BBBB-4A49-8AD0-8628A0367B7C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7857D6-3835-43DA-B4EF-8D8B29DFDB96}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{B9A26406-05FA-4FD5-AABB-5F887CCEE042}"/>
   </bookViews>
@@ -410,7 +410,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,7 +699,7 @@
         <v>43178</v>
       </c>
       <c r="B10">
-        <v>4.25</v>
+        <v>8.25</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -709,7 +709,7 @@
       </c>
       <c r="I10">
         <f t="shared" si="0"/>
-        <v>4.25</v>
+        <v>8.25</v>
       </c>
       <c r="J10" t="s">
         <v>9</v>
@@ -862,7 +862,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f>SUM(I2:I18)</f>
-        <v>272.5</v>
+        <v>276.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Recreated JUnit tests with newer library.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\FinalProject\PRCO304\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7857D6-3835-43DA-B4EF-8D8B29DFDB96}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3940C28B-DA79-4165-902A-06CE444FBFF9}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{B9A26406-05FA-4FD5-AABB-5F887CCEE042}"/>
   </bookViews>
@@ -410,7 +410,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,14 +702,14 @@
         <v>8.25</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="I10">
         <f t="shared" si="0"/>
-        <v>8.25</v>
+        <v>9.75</v>
       </c>
       <c r="J10" t="s">
         <v>9</v>
@@ -862,7 +862,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f>SUM(I2:I18)</f>
-        <v>276.5</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaned Exception caused by MathsHelpers. Finished some tests. Working towards sorting the jTable.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\FinalProject\PRCO304\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3940C28B-DA79-4165-902A-06CE444FBFF9}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8EA9E43-DE9B-4C2A-ABF3-D4B548380EE3}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{B9A26406-05FA-4FD5-AABB-5F887CCEE042}"/>
   </bookViews>
@@ -410,7 +410,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,11 +705,11 @@
         <v>1.5</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="I10">
         <f t="shared" si="0"/>
-        <v>9.75</v>
+        <v>11.25</v>
       </c>
       <c r="J10" t="s">
         <v>9</v>
@@ -862,7 +862,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f>SUM(I2:I18)</f>
-        <v>278</v>
+        <v>279.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working through tests + adjusting classes to handle unexpected/null values as necessary. Remake API after purging of obsolete fields from database.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\FinalProject\PRCO304\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8EA9E43-DE9B-4C2A-ABF3-D4B548380EE3}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC4FD80-2D14-4741-B371-CDC091E56545}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{B9A26406-05FA-4FD5-AABB-5F887CCEE042}"/>
   </bookViews>
@@ -410,7 +410,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,9 +707,12 @@
       <c r="D10">
         <v>1.5</v>
       </c>
+      <c r="E10">
+        <v>4.5</v>
+      </c>
       <c r="I10">
         <f t="shared" si="0"/>
-        <v>11.25</v>
+        <v>15.75</v>
       </c>
       <c r="J10" t="s">
         <v>9</v>
@@ -862,7 +865,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f>SUM(I2:I18)</f>
-        <v>279.5</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
JUnit testing + related fixes for APIControllers.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\FinalProject\PRCO304\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC4FD80-2D14-4741-B371-CDC091E56545}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66994C12-9A08-4B71-8157-EFACE7F23556}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{B9A26406-05FA-4FD5-AABB-5F887CCEE042}"/>
   </bookViews>
@@ -410,7 +410,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,11 +708,14 @@
         <v>1.5</v>
       </c>
       <c r="E10">
-        <v>4.5</v>
+        <v>6.5</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
       </c>
       <c r="I10">
         <f t="shared" si="0"/>
-        <v>15.75</v>
+        <v>22.75</v>
       </c>
       <c r="J10" t="s">
         <v>9</v>
@@ -865,7 +868,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f>SUM(I2:I18)</f>
-        <v>284</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working through tests + changing code to handle exceptions as necessary. Performance tweak for tests where possible.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\FinalProject\PRCO304\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66994C12-9A08-4B71-8157-EFACE7F23556}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98ADF8E9-FA3A-49C7-866A-A2F6DAAEC5A7}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{B9A26406-05FA-4FD5-AABB-5F887CCEE042}"/>
   </bookViews>
@@ -410,7 +410,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,11 +711,11 @@
         <v>6.5</v>
       </c>
       <c r="F10">
-        <v>5</v>
+        <v>6.25</v>
       </c>
       <c r="I10">
         <f t="shared" si="0"/>
-        <v>22.75</v>
+        <v>24</v>
       </c>
       <c r="J10" t="s">
         <v>9</v>
@@ -868,7 +868,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f>SUM(I2:I18)</f>
-        <v>291</v>
+        <v>292.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working through testing. Just a few left and I can get on that neural network *_*
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\FinalProject\PRCO304\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98ADF8E9-FA3A-49C7-866A-A2F6DAAEC5A7}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FD033DF-E469-4611-95F1-4B678C2260CC}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{B9A26406-05FA-4FD5-AABB-5F887CCEE042}"/>
   </bookViews>
@@ -410,7 +410,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,9 +713,15 @@
       <c r="F10">
         <v>6.25</v>
       </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>6</v>
+      </c>
       <c r="I10">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="J10" t="s">
         <v>9</v>
@@ -868,7 +874,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f>SUM(I2:I18)</f>
-        <v>292.25</v>
+        <v>298.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Replaced TradeMode and HoldMode with enums. Work towards final few tests (going to be intensive designs/tests due to nature of algorithms).
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\FinalProject\PRCO304\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FD033DF-E469-4611-95F1-4B678C2260CC}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05EA7010-CEF0-4384-8283-7A621C578635}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{B9A26406-05FA-4FD5-AABB-5F887CCEE042}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -410,7 +410,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,9 +773,21 @@
       <c r="D12">
         <v>0</v>
       </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
       <c r="I12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J12" t="s">
         <v>9</v>
@@ -874,7 +886,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f>SUM(I2:I18)</f>
-        <v>298.25</v>
+        <v>300.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixing issue with GOFAI predictions discovered when junit testing. Should improve prediction accuracy (and therefore profitability)
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\FinalProject\PRCO304\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A904A0-0A11-4493-91DA-88B8AFC75116}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625685C0-991D-4412-9896-540EF536DD58}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{B9A26406-05FA-4FD5-AABB-5F887CCEE042}"/>
   </bookViews>
@@ -410,7 +410,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -783,11 +783,11 @@
         <v>0</v>
       </c>
       <c r="H12">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I12">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J12" t="s">
         <v>9</v>
@@ -886,7 +886,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f>SUM(I2:I18)</f>
-        <v>301.25</v>
+        <v>304.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working way through JavaDoc. Most of the way through Currency.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\FinalProject\PRCO304\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE37C6F9-9672-4F1E-ACD4-63F216D72070}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16057CA5-93D7-48C4-A63A-BDA1A48F13BC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{B9A26406-05FA-4FD5-AABB-5F887CCEE042}"/>
   </bookViews>
@@ -410,7 +410,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -798,7 +798,7 @@
         <v>43199</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -808,7 +808,7 @@
       </c>
       <c r="I13">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -889,7 +889,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f>SUM(I2:I18)</f>
-        <v>310.25</v>
+        <v>312.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working through JavaDoc. Small amount of logic prepared for Neural Network predictions.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\FinalProject\PRCO304\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16057CA5-93D7-48C4-A63A-BDA1A48F13BC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0301B398-9CEA-4BB4-A765-06AE2800F49A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{B9A26406-05FA-4FD5-AABB-5F887CCEE042}"/>
   </bookViews>
@@ -410,7 +410,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,14 +801,14 @@
         <v>8</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
       <c r="I13">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -889,7 +889,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f>SUM(I2:I18)</f>
-        <v>312.25</v>
+        <v>317.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Javadoc finished. JUnit testing finished. Fixed an issue when attempting to buy or sell a cryptocurrency at /usr/bin/bash creating infinite crypto or causing all money to disappear.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\FinalProject\PRCO304\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0301B398-9CEA-4BB4-A765-06AE2800F49A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74257401-FDED-43EE-9280-D35AA206FFDD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{B9A26406-05FA-4FD5-AABB-5F887CCEE042}"/>
   </bookViews>
@@ -410,7 +410,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -804,11 +804,17 @@
         <v>5</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
       </c>
       <c r="I13">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -889,7 +895,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f>SUM(I2:I18)</f>
-        <v>317.25</v>
+        <v>324.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Display times are correctly offset from stored time [UTC] to system LocalDateTime
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\FinalProject\PRCO304\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74257401-FDED-43EE-9280-D35AA206FFDD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9DC896-9E2E-429E-8EA3-F57563E0ECFF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{B9A26406-05FA-4FD5-AABB-5F887CCEE042}"/>
   </bookViews>
@@ -410,7 +410,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="K18" sqref="K18:L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,11 +810,14 @@
         <v>4</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="G13">
+        <v>5</v>
       </c>
       <c r="I13">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -895,7 +898,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f>SUM(I2:I18)</f>
-        <v>324.25</v>
+        <v>330.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating hours worked on UML diagram.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\FinalProject\PRCO304\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9DC896-9E2E-429E-8EA3-F57563E0ECFF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C23BC353-08CD-47CC-8C42-B0FF476F52E9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{B9A26406-05FA-4FD5-AABB-5F887CCEE042}"/>
   </bookViews>
@@ -410,7 +410,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18:L18"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,15 +815,21 @@
       <c r="G13">
         <v>5</v>
       </c>
+      <c r="H13">
+        <v>6</v>
+      </c>
       <c r="I13">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43206</v>
       </c>
+      <c r="B14">
+        <v>6</v>
+      </c>
       <c r="C14">
         <v>0</v>
       </c>
@@ -832,7 +838,7 @@
       </c>
       <c r="I14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -898,7 +904,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f>SUM(I2:I18)</f>
-        <v>330.25</v>
+        <v>342.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UI tweaking. Report work.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\FinalProject\PRCO304\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9DED756-F86D-4795-A9F7-F0F6B396B4AF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D56BA1-61C0-4D9F-A9B3-F8B3C0DE50EE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{B9A26406-05FA-4FD5-AABB-5F887CCEE042}"/>
   </bookViews>
@@ -410,7 +410,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -891,14 +891,14 @@
         <v>7</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
       <c r="I16">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -934,7 +934,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19">
         <f>SUM(I2:I18)</f>
-        <v>403.25</v>
+        <v>404.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added auto-put growth at lap 3. Report work.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\FinalProject\PRCO304\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4332A1CE-B8FC-428A-96ED-803BEC0EAB11}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54AB750-E2F2-4F4F-86D1-C0BB925FA164}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{B9A26406-05FA-4FD5-AABB-5F887CCEE042}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>Week Commencing</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Easter</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -407,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D973A54-FCD3-4BD0-A506-47414655087F}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="C19" sqref="C17:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,7 +543,7 @@
         <v>7.25</v>
       </c>
       <c r="I4">
-        <f t="shared" ref="I4:I18" si="0">SUM(B4:H4)</f>
+        <f t="shared" ref="I4:I17" si="0">SUM(B4:H4)</f>
         <v>36.5</v>
       </c>
     </row>
@@ -902,21 +905,21 @@
       <c r="F16">
         <v>7</v>
       </c>
+      <c r="G16">
+        <v>5</v>
+      </c>
+      <c r="H16">
+        <v>3</v>
+      </c>
       <c r="I16">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43227</v>
       </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
       <c r="I17">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -926,21 +929,33 @@
       <c r="A18" s="1">
         <v>43234</v>
       </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
       <c r="I18">
-        <f t="shared" si="0"/>
+        <f>SUM(B18:H18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>43241</v>
+      </c>
+      <c r="F19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" t="s">
+        <v>10</v>
+      </c>
       <c r="I19">
-        <f>SUM(I2:I18)</f>
-        <v>418.25</v>
+        <f>SUM(B19:E19)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <f>SUM(I2:I19)</f>
+        <v>426.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Report work. Neural Network research. Bug fixes.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\FinalProject\PRCO304\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C5CBAF-BD53-4583-B491-BE844A4470D8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A03673DE-9CFB-40D5-BABC-8DC4509C3D0B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{B9A26406-05FA-4FD5-AABB-5F887CCEE042}"/>
   </bookViews>
@@ -413,7 +413,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,14 +933,17 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="G17">
         <v>7</v>
       </c>
+      <c r="H17">
+        <v>7</v>
+      </c>
       <c r="I17">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>24.5</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -973,7 +976,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I20">
         <f>SUM(I2:I19)</f>
-        <v>443.25</v>
+        <v>450.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Report work. NN research. Tidying application for viva.
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Desktop\FinalProject\PRCO304\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A03673DE-9CFB-40D5-BABC-8DC4509C3D0B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C2079EC-12A5-448A-B1D7-4BFFB72A8843}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{B9A26406-05FA-4FD5-AABB-5F887CCEE042}"/>
   </bookViews>
@@ -413,7 +413,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,9 +950,12 @@
       <c r="A18" s="1">
         <v>43234</v>
       </c>
+      <c r="B18">
+        <v>7</v>
+      </c>
       <c r="I18">
         <f>SUM(B18:H18)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -976,7 +979,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I20">
         <f>SUM(I2:I19)</f>
-        <v>450.75</v>
+        <v>457.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>